<commit_message>
changed diodes in conductivity sensor
</commit_message>
<xml_diff>
--- a/BOM/bom.xlsx
+++ b/BOM/bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="156">
   <si>
     <t>Comment</t>
   </si>
@@ -230,24 +230,15 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>R21, R22, R23, R24</t>
-  </si>
-  <si>
     <t>J1-0603</t>
   </si>
   <si>
     <t>0R</t>
   </si>
   <si>
-    <t>R2, R3</t>
-  </si>
-  <si>
     <t>1K</t>
   </si>
   <si>
-    <t>R20</t>
-  </si>
-  <si>
     <t>1M</t>
   </si>
   <si>
@@ -257,9 +248,6 @@
     <t>Capacitor (Semiconductor SIM Model)</t>
   </si>
   <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>1608[0603]</t>
   </si>
   <si>
@@ -272,12 +260,6 @@
     <t>2.2uF</t>
   </si>
   <si>
-    <t>R_ISET</t>
-  </si>
-  <si>
-    <t>3k</t>
-  </si>
-  <si>
     <t>R7, R8, R9, R10</t>
   </si>
   <si>
@@ -287,12 +269,6 @@
     <t>4.7uF</t>
   </si>
   <si>
-    <t>R1, R4, R6, R18, R25, R26, R27</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
     <t>C8, C9</t>
   </si>
   <si>
@@ -305,9 +281,6 @@
     <t>12pF</t>
   </si>
   <si>
-    <t>R16, R17</t>
-  </si>
-  <si>
     <t>C7, C10, C11, C13, C17, C20, C21, C22</t>
   </si>
   <si>
@@ -320,9 +293,6 @@
     <t>220nF</t>
   </si>
   <si>
-    <t>C16</t>
-  </si>
-  <si>
     <t>470nF</t>
   </si>
   <si>
@@ -332,9 +302,6 @@
     <t>0100020P1</t>
   </si>
   <si>
-    <t>C1, C4, C5, C6, C18</t>
-  </si>
-  <si>
     <t>0100340P1</t>
   </si>
   <si>
@@ -347,9 +314,6 @@
     <t>1.2k 1%</t>
   </si>
   <si>
-    <t xml:space="preserve">100R </t>
-  </si>
-  <si>
     <t>R111, R112</t>
   </si>
   <si>
@@ -360,12 +324,6 @@
   </si>
   <si>
     <t>0011240P1</t>
-  </si>
-  <si>
-    <t>0010010P1</t>
-  </si>
-  <si>
-    <t>22R</t>
   </si>
   <si>
     <t>NA</t>
@@ -475,6 +433,66 @@
   </si>
   <si>
     <t>FC-12M</t>
+  </si>
+  <si>
+    <t>R11, R12, R13, R14, R21, R22, R23, R24</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>100K</t>
+  </si>
+  <si>
+    <t>100R</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>200k</t>
+  </si>
+  <si>
+    <t>27R</t>
+  </si>
+  <si>
+    <t>8.2k</t>
+  </si>
+  <si>
+    <t>R19, R28, R29, R1, R2, R15</t>
+  </si>
+  <si>
+    <t>R18, R25, R26, R27</t>
+  </si>
+  <si>
+    <t>C23, C24</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4, R20</t>
+  </si>
+  <si>
+    <t>C3, C4</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R17, R16</t>
+  </si>
+  <si>
+    <t>C1, C6, C18</t>
+  </si>
+  <si>
+    <t>C5, C16</t>
+  </si>
+  <si>
+    <t>R5</t>
   </si>
 </sst>
 </file>
@@ -619,7 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -667,6 +685,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -948,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A39" sqref="A20:J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,10 +989,10 @@
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="F1" s="34"/>
     </row>
@@ -988,13 +1007,13 @@
         <v>5</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>
@@ -1006,10 +1025,10 @@
         <v>3</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="K2" s="30" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1019,8 +1038,8 @@
       <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>149</v>
+      <c r="C3" s="35" t="s">
+        <v>135</v>
       </c>
       <c r="D3" s="13">
         <v>306010020</v>
@@ -1028,7 +1047,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="2" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>8</v>
@@ -1041,7 +1060,7 @@
         <v>0.79999999999999993</v>
       </c>
       <c r="K3" s="22">
-        <f t="shared" ref="K3:K37" si="0">J3*B3</f>
+        <f>J3*B3</f>
         <v>0.79999999999999993</v>
       </c>
     </row>
@@ -1056,7 +1075,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="13"/>
@@ -1074,25 +1093,25 @@
         <v>0.02</v>
       </c>
       <c r="K4" s="22">
-        <f t="shared" si="0"/>
+        <f>J4*B4</f>
         <v>0.02</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F5" s="32"/>
       <c r="G5" s="2" t="s">
@@ -1102,13 +1121,13 @@
         <v>14</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="J5" s="22">
         <v>1.5</v>
       </c>
       <c r="K5" s="22">
-        <f t="shared" si="0"/>
+        <f>J5*B5</f>
         <v>3</v>
       </c>
     </row>
@@ -1123,14 +1142,14 @@
         <v>7</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E6" s="29"/>
       <c r="F6" s="12" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>16</v>
@@ -1142,7 +1161,7 @@
         <v>0.7</v>
       </c>
       <c r="K6" s="22">
-        <f t="shared" si="0"/>
+        <f>J6*B6</f>
         <v>0.7</v>
       </c>
     </row>
@@ -1157,7 +1176,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="E7" s="24"/>
       <c r="F7" s="23"/>
@@ -1174,7 +1193,7 @@
         <v>31.5</v>
       </c>
       <c r="K7" s="22">
-        <f t="shared" si="0"/>
+        <f>J7*B7</f>
         <v>31.5</v>
       </c>
     </row>
@@ -1207,7 +1226,7 @@
         <v>0.5</v>
       </c>
       <c r="K8" s="22">
-        <f t="shared" si="0"/>
+        <f>J8*B8</f>
         <v>0.5</v>
       </c>
     </row>
@@ -1222,7 +1241,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="23"/>
@@ -1240,7 +1259,7 @@
         <v>0.03</v>
       </c>
       <c r="K9" s="22">
-        <f t="shared" si="0"/>
+        <f>J9*B9</f>
         <v>0.06</v>
       </c>
     </row>
@@ -1255,10 +1274,10 @@
         <v>7</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="2" t="s">
@@ -1274,7 +1293,7 @@
         <v>1.59</v>
       </c>
       <c r="K10" s="22">
-        <f t="shared" si="0"/>
+        <f>J10*B10</f>
         <v>1.59</v>
       </c>
     </row>
@@ -1289,10 +1308,10 @@
         <v>7</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="2" t="s">
@@ -1308,7 +1327,7 @@
         <v>1.24</v>
       </c>
       <c r="K11" s="22">
-        <f t="shared" si="0"/>
+        <f>J11*B11</f>
         <v>1.24</v>
       </c>
     </row>
@@ -1323,11 +1342,11 @@
         <v>7</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E12" s="24"/>
       <c r="F12" s="24" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>37</v>
@@ -1342,7 +1361,7 @@
         <v>3.79</v>
       </c>
       <c r="K12" s="22">
-        <f t="shared" si="0"/>
+        <f>J12*B12</f>
         <v>3.79</v>
       </c>
     </row>
@@ -1357,10 +1376,10 @@
         <v>7</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="2" t="s">
@@ -1376,7 +1395,7 @@
         <v>1.82</v>
       </c>
       <c r="K13" s="22">
-        <f t="shared" si="0"/>
+        <f>J13*B13</f>
         <v>1.82</v>
       </c>
     </row>
@@ -1391,10 +1410,10 @@
         <v>7</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="2" t="s">
@@ -1410,7 +1429,7 @@
         <v>3.15</v>
       </c>
       <c r="K14" s="22">
-        <f t="shared" si="0"/>
+        <f>J14*B14</f>
         <v>3.15</v>
       </c>
     </row>
@@ -1442,13 +1461,13 @@
         <v>39.950000000000003</v>
       </c>
       <c r="K15" s="22">
-        <f t="shared" si="0"/>
+        <f>J15*B15</f>
         <v>39.950000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -1474,7 +1493,7 @@
         <v>3.5</v>
       </c>
       <c r="K16" s="22">
-        <f t="shared" si="0"/>
+        <f>J16*B16</f>
         <v>3.5</v>
       </c>
     </row>
@@ -1489,7 +1508,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="E17" s="24"/>
       <c r="F17" s="23"/>
@@ -1507,7 +1526,7 @@
         <v>0.3</v>
       </c>
       <c r="K17" s="22">
-        <f t="shared" si="0"/>
+        <f>J17*B17</f>
         <v>0.3</v>
       </c>
     </row>
@@ -1522,10 +1541,10 @@
         <v>7</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F18" s="25"/>
       <c r="G18" s="2" t="s">
@@ -1541,7 +1560,7 @@
         <v>0.68</v>
       </c>
       <c r="K18" s="22">
-        <f t="shared" si="0"/>
+        <f>J18*B18</f>
         <v>1.36</v>
       </c>
     </row>
@@ -1556,10 +1575,10 @@
         <v>7</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="2" t="s">
@@ -1575,7 +1594,7 @@
         <v>8.0500000000000007</v>
       </c>
       <c r="K19" s="22">
-        <f t="shared" si="0"/>
+        <f>J19*B19</f>
         <v>8.0500000000000007</v>
       </c>
     </row>
@@ -1584,13 +1603,13 @@
         <v>66</v>
       </c>
       <c r="B20" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E20" s="24"/>
       <c r="F20" s="23"/>
@@ -1598,17 +1617,17 @@
         <v>67</v>
       </c>
       <c r="H20" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="J20" s="22">
         <v>0.01</v>
       </c>
       <c r="K20" s="22">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
+        <f>J20*B20</f>
+        <v>0.08</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1616,13 +1635,13 @@
         <v>66</v>
       </c>
       <c r="B21" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>105</v>
+        <v>95</v>
+      </c>
+      <c r="D21" s="13">
+        <v>301010206</v>
       </c>
       <c r="E21" s="24"/>
       <c r="F21" s="23"/>
@@ -1630,81 +1649,79 @@
         <v>67</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J21" s="22">
         <v>0.01</v>
       </c>
       <c r="K21" s="22">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
+        <f>J21*B21</f>
+        <v>0.01</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>66</v>
+        <v>137</v>
       </c>
       <c r="B22" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="13">
-        <v>301010151</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="D22" s="13"/>
       <c r="E22" s="24"/>
       <c r="F22" s="23"/>
       <c r="G22" s="2" t="s">
         <v>67</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>73</v>
+        <v>145</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J22" s="22">
         <v>0.01</v>
       </c>
       <c r="K22" s="22">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
+        <f t="shared" ref="K22:K39" si="0">J22*B22</f>
+        <v>0.06</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B23" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" s="24"/>
+        <v>91</v>
+      </c>
+      <c r="E23" s="23"/>
       <c r="F23" s="23"/>
       <c r="G23" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J23" s="22">
         <v>0.05</v>
       </c>
       <c r="K23" s="22">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1712,13 +1729,13 @@
         <v>66</v>
       </c>
       <c r="B24" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="D24" s="13">
-        <v>301010206</v>
+        <v>301010090</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="23"/>
@@ -1726,17 +1743,17 @@
         <v>67</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J24" s="22">
         <v>0.01</v>
       </c>
       <c r="K24" s="22">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1744,13 +1761,13 @@
         <v>66</v>
       </c>
       <c r="B25" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" s="13">
-        <v>301010090</v>
+        <v>140</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="23"/>
@@ -1758,145 +1775,143 @@
         <v>67</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J25" s="22">
         <v>0.01</v>
       </c>
       <c r="K25" s="22">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B26" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D26" s="13">
-        <v>301010170</v>
-      </c>
-      <c r="E26" s="24"/>
+        <v>302010001</v>
+      </c>
+      <c r="E26" s="23"/>
       <c r="F26" s="23"/>
       <c r="G26" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J26" s="22">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="K26" s="22">
         <f t="shared" si="0"/>
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B27" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="E27" s="24"/>
+        <v>141</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="E27" s="23"/>
       <c r="F27" s="23"/>
       <c r="G27" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>84</v>
+        <v>147</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="J27" s="22">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="K27" s="22">
         <f t="shared" si="0"/>
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B28" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D28" s="13">
-        <v>302010054</v>
-      </c>
-      <c r="E28" s="24"/>
+        <v>302010067</v>
+      </c>
+      <c r="E28" s="23"/>
       <c r="F28" s="23"/>
       <c r="G28" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J28" s="22">
         <v>0.05</v>
       </c>
       <c r="K28" s="22">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B29" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="13">
-        <v>302010111</v>
+        <v>70</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="E29" s="24"/>
       <c r="F29" s="23"/>
       <c r="G29" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>102</v>
+        <v>148</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="J29" s="22">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="K29" s="22">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1904,13 +1919,13 @@
         <v>66</v>
       </c>
       <c r="B30" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>111</v>
+        <v>71</v>
+      </c>
+      <c r="D30" s="13">
+        <v>301010151</v>
       </c>
       <c r="E30" s="24"/>
       <c r="F30" s="23"/>
@@ -1918,42 +1933,42 @@
         <v>67</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>87</v>
+        <v>149</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J30" s="22">
         <v>0.01</v>
       </c>
       <c r="K30" s="22">
         <f t="shared" si="0"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B31" s="3">
         <v>2</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D31" s="13">
-        <v>302010001</v>
-      </c>
-      <c r="E31" s="23"/>
+        <v>75</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="24"/>
       <c r="F31" s="23"/>
       <c r="G31" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J31" s="22">
         <v>0.05</v>
@@ -1965,34 +1980,34 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B32" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="D32" s="13">
-        <v>302010067</v>
-      </c>
-      <c r="E32" s="23"/>
+        <v>302010054</v>
+      </c>
+      <c r="E32" s="24"/>
       <c r="F32" s="23"/>
       <c r="G32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="I32" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J32" s="22">
         <v>0.05</v>
       </c>
       <c r="K32" s="22">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2000,215 +2015,308 @@
         <v>66</v>
       </c>
       <c r="B33" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E33" s="23"/>
+        <v>142</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="24"/>
       <c r="F33" s="23"/>
       <c r="G33" s="2" t="s">
         <v>67</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>93</v>
+        <v>151</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J33" s="22">
         <v>0.01</v>
       </c>
       <c r="K33" s="22">
         <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B34" s="3">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>101</v>
+        <v>88</v>
+      </c>
+      <c r="D34" s="13">
+        <v>302010073</v>
       </c>
       <c r="E34" s="23"/>
       <c r="F34" s="23"/>
       <c r="G34" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J34" s="22">
         <v>0.05</v>
       </c>
       <c r="K34" s="22">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B35" s="3">
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D35" s="13">
-        <v>302010073</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D35" s="13"/>
       <c r="E35" s="23"/>
       <c r="F35" s="23"/>
       <c r="G35" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>96</v>
+        <v>152</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="J35" s="22">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="K35" s="22">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B36" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="D36" s="13">
-        <v>302010092</v>
-      </c>
-      <c r="E36" s="23"/>
+        <v>302010111</v>
+      </c>
+      <c r="E36" s="24"/>
       <c r="F36" s="23"/>
       <c r="G36" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J36" s="22">
         <v>0.05</v>
       </c>
       <c r="K36" s="22">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.15000000000000002</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="B37" s="18">
-        <v>1</v>
-      </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="19" t="s">
-        <v>126</v>
+      <c r="A37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="3">
+        <v>2</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="13">
+        <v>302010092</v>
       </c>
       <c r="E37" s="23"/>
       <c r="F37" s="23"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
+      <c r="G37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="J37" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="K37" s="22">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="3">
+        <v>4</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E38" s="24"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J38" s="22">
+        <v>0.01</v>
+      </c>
+      <c r="K38" s="22">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D39" s="13"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J39" s="22">
+        <v>0.01</v>
+      </c>
+      <c r="K39" s="22">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" s="18">
+        <v>1</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="22">
         <f>3/20</f>
         <v>0.15</v>
       </c>
-      <c r="K37" s="22">
-        <f t="shared" si="0"/>
+      <c r="K40" s="22">
+        <f>J40*B40</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I38" s="12"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I39" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="J39" s="22">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I41" s="12"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I42" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="J42" s="22">
         <f>20/5</f>
         <v>4</v>
       </c>
-      <c r="K39" s="22">
-        <f>J39</f>
+      <c r="K42" s="22">
+        <f>J42</f>
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I40" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22">
-        <f>SUM(K3:K39)</f>
-        <v>106.81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
-      <c r="B41" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" t="s">
-        <v>139</v>
-      </c>
-    </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" t="s">
-        <v>121</v>
+      <c r="I43" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22">
+        <f>SUM(K3:K42)</f>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
+      <c r="A44" s="28"/>
       <c r="B44" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>114</v>
-      </c>
+      <c r="A45" s="5"/>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A21:K36">
+    <sortCondition ref="C21:C36"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="E1:F1"/>
   </mergeCells>

</xml_diff>